<commit_message>
refactor: remove deprecated Excel file generator and related configurations
</commit_message>
<xml_diff>
--- a/Excel File Generator/excel-generator/bank-data-text-with-quotePrefix.xlsx
+++ b/Excel File Generator/excel-generator/bank-data-text-with-quotePrefix.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -432,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
@@ -441,73 +441,59 @@
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>